<commit_message>
Add statistical analysis for most plots
</commit_message>
<xml_diff>
--- a/raw-data/P0_Bmp7_symmetry.xlsx
+++ b/raw-data/P0_Bmp7_symmetry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmrot\Documents\R\Bmp7-ins\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAED1C94-37E3-48F3-9145-512F8B328368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6982ED8D-1D67-4A20-B316-53904E6ACE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="16200" windowWidth="14610" windowHeight="7110" xr2:uid="{CAF0392F-C42E-44C2-A774-7DEE11F29449}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CAF0392F-C42E-44C2-A774-7DEE11F29449}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>unnorm_ratio</t>
+  </si>
+  <si>
+    <t>DAPI_ratio</t>
   </si>
 </sst>
 </file>
@@ -434,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF93241-7319-44D9-B0BB-3BE4BE6224F6}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +473,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1681</v>
       </c>
@@ -503,8 +509,12 @@
         <f>C2/F2</f>
         <v>0.89250080463469583</v>
       </c>
+      <c r="J2">
+        <f>E2/B2</f>
+        <v>0.95306638508350239</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1493</v>
       </c>
@@ -529,15 +539,19 @@
         <v>0.15981843533984039</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H4" si="2">D3/G3</f>
+        <f t="shared" ref="H3" si="2">D3/G3</f>
         <v>0.59105622225697119</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I4" si="3">C3/F3</f>
+        <f t="shared" ref="I3" si="3">C3/F3</f>
         <v>0.53127900501206615</v>
       </c>
+      <c r="J3">
+        <f>B3/E3</f>
+        <v>0.89886373750259585</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1503</v>
       </c>
@@ -568,6 +582,10 @@
       <c r="I4">
         <f>F4/C4</f>
         <v>0.81506655338431044</v>
+      </c>
+      <c r="J4">
+        <f>B4/E4</f>
+        <v>0.98729416404896397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>